<commit_message>
mais abas e evolução incluida
</commit_message>
<xml_diff>
--- a/Arrecadacao Tributos.xlsx
+++ b/Arrecadacao Tributos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sistemas Prefeitura\WEB\Dashboard Tributos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D657047-10AC-4228-9875-130442330A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72CCF2AE-A0DA-4DAA-AC64-466A507C3019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,7 +113,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -136,17 +136,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -155,17 +144,17 @@
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -450,7 +439,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,163 +452,163 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>2020</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>56049554.979999997</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>101557275.95999999</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>21646657.43</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="5">
         <v>5720152.5</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <f>SUM(B4:E4)</f>
         <v>184973640.87</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>2021</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>72598444.799999997</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>118375211.58</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>32375582.68</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="5">
         <v>6851258.1699999999</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <f t="shared" ref="F5:F8" si="0">SUM(B5:E5)</f>
         <v>230200497.22999999</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>2022</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>78402847</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>147708693.15000001</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>39953311.649999999</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="5">
         <v>7437047.6799999997</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <f t="shared" si="0"/>
         <v>273501899.48000002</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>2023</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>102619949.78</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>175588791.37</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>35813419.439999998</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="5">
         <v>8278342.3099999996</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <f t="shared" si="0"/>
         <v>322300502.89999998</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>2024</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>117706601.12</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>210718537.03</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>42989074.280000001</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="5">
         <v>8922314.1699999999</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <f t="shared" si="0"/>
         <v>380336526.59999996</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>2025</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="7">
         <v>86562567.810000002</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>109561210.54000001</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>29548040.030000001</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>9041719.5199999996</v>
       </c>
-      <c r="F9" s="4">
-        <f>SUM(C9:E9)</f>
-        <v>148150970.09</v>
+      <c r="F9" s="3">
+        <f>SUM(B9:E9)</f>
+        <v>234713537.90000004</v>
       </c>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
+      <c r="B10" s="8"/>
       <c r="F10" s="1"/>
     </row>
   </sheetData>

</xml_diff>